<commit_message>
Excel and 2 maps
map
balance
</commit_message>
<xml_diff>
--- a/Assets/Data/Characteristics.xlsx
+++ b/Assets/Data/Characteristics.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Clash-Mini\Assets\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F08011A3-418C-48FF-9C9A-190F104344DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC008D56-3224-4B25-BE19-C8DAE0B5ADC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
   <si>
     <t>Имя персонажа</t>
   </si>
@@ -138,13 +138,25 @@
   </si>
   <si>
     <t>Enemy Strenght</t>
+  </si>
+  <si>
+    <t>for me</t>
+  </si>
+  <si>
+    <t>4=== 7</t>
+  </si>
+  <si>
+    <t>7===…...</t>
+  </si>
+  <si>
+    <t>1===4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,8 +201,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -222,8 +241,13 @@
         <fgColor rgb="FFA5A5A5"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -261,30 +285,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="5"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="6" applyFont="1"/>
+    <xf numFmtId="16" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
     <cellStyle name="Check Cell" xfId="5" builtinId="23"/>
     <cellStyle name="Good" xfId="3" builtinId="26"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="6" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -619,7 +662,7 @@
   <dimension ref="A1:S166"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,6 +678,8 @@
     <col min="9" max="9" width="13.28515625" customWidth="1"/>
     <col min="10" max="10" width="18.28515625" customWidth="1"/>
     <col min="11" max="11" width="17.140625" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" customWidth="1"/>
+    <col min="14" max="14" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -671,6 +716,9 @@
       <c r="K1" t="s">
         <v>33</v>
       </c>
+      <c r="L1" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -678,7 +726,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C3">
         <v>25</v>
@@ -692,22 +740,28 @@
       <c r="F3">
         <v>1000</v>
       </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3" s="3">
+      <c r="G3" s="6">
+        <v>0</v>
+      </c>
+      <c r="H3">
         <v>5</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="3">
         <f>C3/D3</f>
         <v>25</v>
       </c>
       <c r="J3">
         <v>1</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="3">
         <f>(B3/60+I3/25+E3/50)*J3</f>
-        <v>2.8333333333333335</v>
+        <v>3</v>
+      </c>
+      <c r="L3" s="2">
+        <v>2.8</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -721,7 +775,7 @@
         <v>25</v>
       </c>
       <c r="D4" s="4">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="E4">
         <v>60</v>
@@ -729,22 +783,28 @@
       <c r="F4">
         <v>1000</v>
       </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4" s="3">
+      <c r="G4" s="6">
+        <v>0</v>
+      </c>
+      <c r="H4">
         <v>5</v>
       </c>
-      <c r="I4">
-        <f t="shared" ref="I4:I38" si="0">C4/D4</f>
-        <v>25</v>
+      <c r="I4" s="3">
+        <f t="shared" ref="I4:I13" si="0">C4/D4</f>
+        <v>19.23076923076923</v>
       </c>
       <c r="J4">
         <v>1</v>
       </c>
-      <c r="K4">
-        <f t="shared" ref="K4:K27" si="1">(B4/60+I4/25+E4/50)*J4</f>
-        <v>2.8666666666666663</v>
+      <c r="K4" s="3">
+        <f t="shared" ref="K4:K13" si="1">(B4/60+I4/25+E4/50)*J4</f>
+        <v>2.6358974358974354</v>
+      </c>
+      <c r="L4" s="2">
+        <v>2.8</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -758,7 +818,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="E5">
         <v>50</v>
@@ -766,22 +826,28 @@
       <c r="F5">
         <v>1000</v>
       </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5" s="3">
+      <c r="G5" s="6">
+        <v>0</v>
+      </c>
+      <c r="H5">
         <v>3</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="3">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>12.5</v>
       </c>
       <c r="J5">
         <v>3</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="3">
         <f t="shared" si="1"/>
-        <v>5.45</v>
+        <v>5.75</v>
+      </c>
+      <c r="L5" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -795,7 +861,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="4">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="E6">
         <v>40</v>
@@ -803,22 +869,25 @@
       <c r="F6">
         <v>1000</v>
       </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6" s="3">
+      <c r="G6" s="6">
+        <v>0</v>
+      </c>
+      <c r="H6">
         <v>2</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="3">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>5.5555555555555554</v>
       </c>
       <c r="J6">
         <v>5</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="3">
         <f t="shared" si="1"/>
-        <v>6.6666666666666679</v>
+        <v>6.7777777777777786</v>
+      </c>
+      <c r="L6" s="1">
+        <v>6.6</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -832,7 +901,7 @@
         <v>30</v>
       </c>
       <c r="D7" s="4">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="E7">
         <v>35</v>
@@ -840,22 +909,25 @@
       <c r="F7">
         <v>1000</v>
       </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7" s="3">
+      <c r="G7" s="6">
+        <v>0</v>
+      </c>
+      <c r="H7">
         <v>6</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="3">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J7">
         <v>1</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="3">
         <f t="shared" si="1"/>
-        <v>3.2333333333333334</v>
+        <v>3.0333333333333332</v>
+      </c>
+      <c r="L7" s="5">
+        <v>3.2</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -877,22 +949,25 @@
       <c r="F8">
         <v>1000</v>
       </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8" s="3">
+      <c r="G8" s="6">
+        <v>0</v>
+      </c>
+      <c r="H8">
         <v>4</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="J8">
         <v>3</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="3">
         <f t="shared" si="1"/>
         <v>6.6000000000000005</v>
+      </c>
+      <c r="L8" s="1">
+        <v>6.6</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -906,7 +981,7 @@
         <v>50</v>
       </c>
       <c r="D9" s="4">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E9">
         <v>30</v>
@@ -914,22 +989,25 @@
       <c r="F9">
         <v>1000</v>
       </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9" s="3">
+      <c r="G9" s="6">
+        <v>0</v>
+      </c>
+      <c r="H9">
         <v>10</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="3">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>33.333333333333336</v>
       </c>
       <c r="J9">
         <v>1</v>
       </c>
-      <c r="K9">
-        <f>(B9/60+I9/25+E9/50)*J9</f>
-        <v>4.2666666666666666</v>
+      <c r="K9" s="3">
+        <f t="shared" si="1"/>
+        <v>3.6</v>
+      </c>
+      <c r="L9" s="5">
+        <v>4.2</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -937,36 +1015,39 @@
         <v>17</v>
       </c>
       <c r="B10">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="C10">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D10" s="4">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="E10">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F10">
         <v>1000</v>
       </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10" s="3">
-        <v>7</v>
-      </c>
-      <c r="I10">
+      <c r="G10" s="6">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>10</v>
+      </c>
+      <c r="I10" s="3">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>3.8461538461538458</v>
       </c>
       <c r="J10">
         <v>6</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="3">
         <f t="shared" si="1"/>
-        <v>13.100000000000001</v>
+        <v>7.2230769230769241</v>
+      </c>
+      <c r="L10" s="2">
+        <v>7.5</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -980,7 +1061,7 @@
         <v>40</v>
       </c>
       <c r="D11" s="4">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="E11">
         <v>60</v>
@@ -988,21 +1069,24 @@
       <c r="F11">
         <v>1000</v>
       </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11" s="3">
+      <c r="G11" s="6">
+        <v>0</v>
+      </c>
+      <c r="H11">
         <v>5</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="3">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>33.333333333333336</v>
       </c>
       <c r="J11">
         <v>2</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="3">
         <f t="shared" si="1"/>
+        <v>5.5666666666666664</v>
+      </c>
+      <c r="L11" s="2">
         <v>6.1</v>
       </c>
     </row>
@@ -1017,7 +1101,7 @@
         <v>45</v>
       </c>
       <c r="D12" s="4">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="E12">
         <v>35</v>
@@ -1025,21 +1109,24 @@
       <c r="F12">
         <v>1000</v>
       </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12" s="3">
+      <c r="G12" s="6">
+        <v>0</v>
+      </c>
+      <c r="H12">
         <v>10</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="3">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="J12">
         <v>1</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="3">
         <f t="shared" si="1"/>
+        <v>5.2</v>
+      </c>
+      <c r="L12" s="5">
         <v>4</v>
       </c>
     </row>
@@ -1062,22 +1149,25 @@
       <c r="F13">
         <v>1000</v>
       </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13" s="3">
+      <c r="G13" s="6">
+        <v>0</v>
+      </c>
+      <c r="H13">
         <v>4</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="3">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="J13">
         <v>3</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="3">
         <f t="shared" si="1"/>
         <v>10.399999999999999</v>
+      </c>
+      <c r="L13" s="2">
+        <v>10.4</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1141,7 +1231,7 @@
       </c>
     </row>
     <row r="16" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>22</v>
       </c>
@@ -1152,7 +1242,7 @@
         <v>55</v>
       </c>
       <c r="D17" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="E17">
         <v>65</v>
@@ -1160,26 +1250,29 @@
       <c r="F17">
         <v>1000</v>
       </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17" s="3">
+      <c r="G17" s="6">
+        <v>0</v>
+      </c>
+      <c r="H17">
         <v>10</v>
       </c>
-      <c r="I17">
-        <f t="shared" si="0"/>
-        <v>55</v>
+      <c r="I17" s="3">
+        <f t="shared" ref="I4:I38" si="2">C17/D17</f>
+        <v>68.75</v>
       </c>
       <c r="J17">
         <v>1</v>
       </c>
-      <c r="K17">
-        <f t="shared" si="1"/>
-        <v>4.833333333333333</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
+      <c r="K17" s="3">
+        <f t="shared" ref="K4:K27" si="3">(B17/60+I17/25+E17/50)*J17</f>
+        <v>5.3833333333333329</v>
+      </c>
+      <c r="L17" s="5">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B18">
@@ -1189,7 +1282,7 @@
         <v>10</v>
       </c>
       <c r="D18" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E18">
         <v>20</v>
@@ -1197,25 +1290,28 @@
       <c r="F18">
         <v>1000</v>
       </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18" s="3">
+      <c r="G18" s="6">
+        <v>0</v>
+      </c>
+      <c r="H18">
         <v>8</v>
       </c>
-      <c r="I18">
-        <f t="shared" si="0"/>
-        <v>10</v>
+      <c r="I18" s="3">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="J18">
         <v>1</v>
       </c>
-      <c r="K18">
-        <f t="shared" si="1"/>
+      <c r="K18" s="3">
+        <f t="shared" si="3"/>
+        <v>3.1</v>
+      </c>
+      <c r="L18" s="2">
         <v>3.3</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
@@ -1226,7 +1322,7 @@
         <v>5</v>
       </c>
       <c r="D19" s="4">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="E19">
         <v>80</v>
@@ -1234,25 +1330,28 @@
       <c r="F19">
         <v>1000</v>
       </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19" s="3">
+      <c r="G19" s="6">
+        <v>0</v>
+      </c>
+      <c r="H19">
         <v>2</v>
       </c>
-      <c r="I19">
-        <f t="shared" si="0"/>
-        <v>5</v>
+      <c r="I19" s="3">
+        <f t="shared" si="2"/>
+        <v>25</v>
       </c>
       <c r="J19">
         <v>3</v>
       </c>
-      <c r="K19">
-        <f t="shared" si="1"/>
-        <v>6.15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K19" s="3">
+        <f t="shared" si="3"/>
+        <v>8.5500000000000007</v>
+      </c>
+      <c r="L19" s="1">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>25</v>
       </c>
@@ -1271,25 +1370,28 @@
       <c r="F20">
         <v>1000</v>
       </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20" s="3">
+      <c r="G20" s="6">
+        <v>0</v>
+      </c>
+      <c r="H20">
         <v>5</v>
       </c>
-      <c r="I20">
-        <f t="shared" si="0"/>
+      <c r="I20" s="3">
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="J20">
         <v>2</v>
       </c>
-      <c r="K20">
-        <f t="shared" si="1"/>
+      <c r="K20" s="3">
+        <f t="shared" si="3"/>
         <v>5.7666666666666666</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L20" s="2">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>26</v>
       </c>
@@ -1308,25 +1410,28 @@
       <c r="F21">
         <v>1000</v>
       </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21" s="3">
+      <c r="G21" s="6">
+        <v>0</v>
+      </c>
+      <c r="H21">
         <v>7</v>
       </c>
-      <c r="I21">
-        <f t="shared" si="0"/>
+      <c r="I21" s="3">
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="J21">
         <v>5</v>
       </c>
-      <c r="K21">
-        <f t="shared" si="1"/>
+      <c r="K21" s="3">
+        <f t="shared" si="3"/>
         <v>9.5833333333333321</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L21" s="1">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>27</v>
       </c>
@@ -1337,7 +1442,7 @@
         <v>40</v>
       </c>
       <c r="D22" s="4">
-        <v>1</v>
+        <v>1.4</v>
       </c>
       <c r="E22">
         <v>35</v>
@@ -1345,25 +1450,28 @@
       <c r="F22">
         <v>1000</v>
       </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22" s="3">
+      <c r="G22" s="6">
+        <v>0</v>
+      </c>
+      <c r="H22">
         <v>9</v>
       </c>
-      <c r="I22">
-        <f t="shared" si="0"/>
-        <v>40</v>
+      <c r="I22" s="3">
+        <f t="shared" si="2"/>
+        <v>28.571428571428573</v>
       </c>
       <c r="J22">
         <v>1</v>
       </c>
-      <c r="K22">
-        <f t="shared" si="1"/>
-        <v>3.55</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K22" s="3">
+        <f t="shared" si="3"/>
+        <v>3.0928571428571434</v>
+      </c>
+      <c r="L22" s="5">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>28</v>
       </c>
@@ -1374,7 +1482,7 @@
         <v>35</v>
       </c>
       <c r="D23" s="4">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="E23">
         <v>40</v>
@@ -1382,25 +1490,28 @@
       <c r="F23">
         <v>1000</v>
       </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23" s="3">
+      <c r="G23" s="6">
+        <v>0</v>
+      </c>
+      <c r="H23">
         <v>7</v>
       </c>
-      <c r="I23">
-        <f t="shared" si="0"/>
-        <v>35</v>
+      <c r="I23" s="3">
+        <f t="shared" si="2"/>
+        <v>26.923076923076923</v>
       </c>
       <c r="J23">
         <v>2</v>
       </c>
-      <c r="K23">
-        <f t="shared" si="1"/>
-        <v>6.0666666666666664</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K23" s="3">
+        <f t="shared" si="3"/>
+        <v>5.4205128205128208</v>
+      </c>
+      <c r="L23" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>29</v>
       </c>
@@ -1419,25 +1530,28 @@
       <c r="F24">
         <v>1000</v>
       </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-      <c r="H24" s="3">
+      <c r="G24" s="6">
+        <v>0</v>
+      </c>
+      <c r="H24">
         <v>9</v>
       </c>
-      <c r="I24">
-        <f t="shared" si="0"/>
+      <c r="I24" s="3">
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="J24">
         <v>1</v>
       </c>
-      <c r="K24">
-        <f t="shared" si="1"/>
+      <c r="K24" s="3">
+        <f t="shared" si="3"/>
         <v>4.2833333333333332</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L24" s="5">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>30</v>
       </c>
@@ -1448,7 +1562,7 @@
         <v>25</v>
       </c>
       <c r="D25" s="4">
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="E25">
         <v>30</v>
@@ -1456,25 +1570,28 @@
       <c r="F25">
         <v>1000</v>
       </c>
-      <c r="G25">
-        <v>0</v>
-      </c>
-      <c r="H25" s="3">
+      <c r="G25" s="6">
+        <v>0</v>
+      </c>
+      <c r="H25">
         <v>5</v>
       </c>
-      <c r="I25">
-        <f t="shared" si="0"/>
-        <v>25</v>
+      <c r="I25" s="3">
+        <f t="shared" si="2"/>
+        <v>15.625</v>
       </c>
       <c r="J25">
         <v>1</v>
       </c>
-      <c r="K25">
-        <f t="shared" si="1"/>
-        <v>2.2666666666666666</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K25" s="3">
+        <f t="shared" si="3"/>
+        <v>1.8916666666666666</v>
+      </c>
+      <c r="L25" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>31</v>
       </c>
@@ -1485,7 +1602,7 @@
         <v>30</v>
       </c>
       <c r="D26" s="4">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="E26">
         <v>65</v>
@@ -1493,25 +1610,28 @@
       <c r="F26">
         <v>1000</v>
       </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
-      <c r="H26" s="3">
+      <c r="G26" s="6">
+        <v>0</v>
+      </c>
+      <c r="H26">
         <v>4</v>
       </c>
-      <c r="I26">
-        <f t="shared" si="0"/>
-        <v>30</v>
+      <c r="I26" s="3">
+        <f t="shared" si="2"/>
+        <v>42.857142857142861</v>
       </c>
       <c r="J26">
         <v>2</v>
       </c>
-      <c r="K26">
-        <f t="shared" si="1"/>
-        <v>6.6666666666666661</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K26" s="3">
+        <f t="shared" si="3"/>
+        <v>7.6952380952380963</v>
+      </c>
+      <c r="L26" s="1">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>32</v>
       </c>
@@ -1525,660 +1645,1077 @@
         <v>10000</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27">
         <v>15</v>
       </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
-      <c r="H27" s="3">
+      <c r="G27" s="6">
+        <v>0</v>
+      </c>
+      <c r="H27">
         <v>6</v>
       </c>
-      <c r="I27">
-        <f t="shared" si="0"/>
+      <c r="I27" s="3">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J27">
         <v>1</v>
       </c>
-      <c r="K27">
-        <f t="shared" si="1"/>
-        <v>4.166666666666667</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K27" s="3">
+        <f t="shared" si="3"/>
+        <v>4.1866666666666665</v>
+      </c>
+      <c r="L27" s="2">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D28" s="4">
         <v>1</v>
       </c>
-      <c r="H28" s="3"/>
-      <c r="I28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G28" s="6">
+        <v>0</v>
+      </c>
+      <c r="I28" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K28" s="3"/>
+    </row>
+    <row r="29" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D29" s="4">
         <v>1</v>
       </c>
-      <c r="H29" s="3"/>
-      <c r="I29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G29" s="6">
+        <v>0</v>
+      </c>
+      <c r="I29" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K29" s="3"/>
+    </row>
+    <row r="30" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D30" s="4">
         <v>1</v>
       </c>
-      <c r="H30" s="3"/>
-      <c r="I30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G30" s="6">
+        <v>0</v>
+      </c>
+      <c r="I30" s="3">
+        <f>C30/D30</f>
+        <v>0</v>
+      </c>
+      <c r="K30" s="3"/>
+    </row>
+    <row r="31" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D31" s="4">
         <v>1</v>
       </c>
-      <c r="H31" s="3"/>
-      <c r="I31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G31" s="6">
+        <v>0</v>
+      </c>
+      <c r="I31" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K31" s="3"/>
+    </row>
+    <row r="32" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D32" s="4">
         <v>1</v>
       </c>
-      <c r="H32" s="3"/>
-      <c r="I32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G32" s="6">
+        <v>0</v>
+      </c>
+      <c r="I32" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K32" s="3"/>
+    </row>
+    <row r="33" spans="2:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33">
         <f>AVERAGE(B18:B27,B17,B3:B13)</f>
-        <v>61.81818181818182</v>
+        <v>61.363636363636367</v>
       </c>
       <c r="C33">
         <f>AVERAGE(B33,C3,C4,C6,C5,C8,C7,C9:C13,C17:C27)</f>
-        <v>28.122529644268774</v>
+        <v>27.66798418972332</v>
       </c>
       <c r="D33" s="4">
         <v>1</v>
       </c>
       <c r="E33">
         <f>AVERAGE(D33,E17:E26,E3:E13)</f>
-        <v>47.31818181818182</v>
-      </c>
-      <c r="H33" s="3"/>
+        <v>46.863636363636367</v>
+      </c>
+      <c r="G33" s="6">
+        <v>0</v>
+      </c>
       <c r="I33">
         <f>AVERAGE(I3,I3:I13,I17:I26)</f>
-        <v>27.727272727272727</v>
-      </c>
-    </row>
-    <row r="34" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>27.751172438672437</v>
+      </c>
+      <c r="K33" s="3"/>
+    </row>
+    <row r="34" spans="2:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D34" s="4">
         <v>1</v>
       </c>
-      <c r="H34" s="3"/>
+      <c r="G34" s="6">
+        <v>0</v>
+      </c>
       <c r="I34">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K34" s="3"/>
+    </row>
+    <row r="35" spans="2:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D35" s="4">
         <v>1</v>
       </c>
-      <c r="H35" s="3"/>
+      <c r="G35" s="6">
+        <v>0</v>
+      </c>
       <c r="I35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K35" s="3"/>
+    </row>
+    <row r="36" spans="2:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D36" s="4">
         <v>1</v>
       </c>
-      <c r="H36" s="3"/>
+      <c r="G36" s="6">
+        <v>0</v>
+      </c>
       <c r="I36">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K36" s="3"/>
+    </row>
+    <row r="37" spans="2:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D37" s="4">
         <v>1</v>
       </c>
-      <c r="H37" s="3"/>
+      <c r="G37" s="6">
+        <v>0</v>
+      </c>
       <c r="I37">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K37" s="3"/>
+    </row>
+    <row r="38" spans="2:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D38" s="4">
         <v>1</v>
       </c>
-      <c r="H38" s="3"/>
+      <c r="G38" s="6">
+        <v>0</v>
+      </c>
       <c r="I38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K38" s="3"/>
+    </row>
+    <row r="39" spans="2:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D39" s="4"/>
-      <c r="H39" s="3"/>
-    </row>
-    <row r="40" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G39" s="6">
+        <v>0</v>
+      </c>
+      <c r="K39" s="3"/>
+    </row>
+    <row r="40" spans="2:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D40" s="4"/>
-      <c r="H40" s="3"/>
-    </row>
-    <row r="41" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G40" s="6">
+        <v>0</v>
+      </c>
+      <c r="K40" s="3"/>
+    </row>
+    <row r="41" spans="2:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D41" s="4"/>
-      <c r="H41" s="3"/>
-    </row>
-    <row r="42" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G41" s="6">
+        <v>0</v>
+      </c>
+      <c r="K41" s="3"/>
+    </row>
+    <row r="42" spans="2:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D42" s="4"/>
-      <c r="H42" s="3"/>
-    </row>
-    <row r="43" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G42" s="6">
+        <v>0</v>
+      </c>
+      <c r="K42" s="3"/>
+    </row>
+    <row r="43" spans="2:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D43" s="4"/>
-      <c r="H43" s="3"/>
-    </row>
-    <row r="44" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G43" s="6">
+        <v>0</v>
+      </c>
+      <c r="K43" s="3"/>
+    </row>
+    <row r="44" spans="2:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D44" s="4"/>
-      <c r="H44" s="3"/>
-    </row>
-    <row r="45" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G44" s="6">
+        <v>0</v>
+      </c>
+      <c r="K44" s="3"/>
+    </row>
+    <row r="45" spans="2:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D45" s="4"/>
-      <c r="H45" s="3"/>
-    </row>
-    <row r="46" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G45" s="6">
+        <v>0</v>
+      </c>
+      <c r="K45" s="3"/>
+    </row>
+    <row r="46" spans="2:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D46" s="4"/>
-      <c r="H46" s="3"/>
-    </row>
-    <row r="47" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G46" s="6">
+        <v>0</v>
+      </c>
+      <c r="K46" s="3"/>
+    </row>
+    <row r="47" spans="2:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D47" s="4"/>
-      <c r="H47" s="3"/>
-    </row>
-    <row r="48" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G47" s="6">
+        <v>0</v>
+      </c>
+      <c r="K47" s="3"/>
+    </row>
+    <row r="48" spans="2:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D48" s="4"/>
-      <c r="H48" s="3"/>
-    </row>
-    <row r="49" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G48" s="6">
+        <v>0</v>
+      </c>
+      <c r="K48" s="3"/>
+    </row>
+    <row r="49" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D49" s="4"/>
-      <c r="H49" s="3"/>
-    </row>
-    <row r="50" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G49" s="6">
+        <v>0</v>
+      </c>
+      <c r="K49" s="3"/>
+    </row>
+    <row r="50" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D50" s="4"/>
-      <c r="H50" s="3"/>
-    </row>
-    <row r="51" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G50" s="6">
+        <v>0</v>
+      </c>
+      <c r="K50" s="3"/>
+    </row>
+    <row r="51" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D51" s="4"/>
-      <c r="H51" s="3"/>
-    </row>
-    <row r="52" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G51" s="6">
+        <v>0</v>
+      </c>
+      <c r="K51" s="3"/>
+    </row>
+    <row r="52" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D52" s="4"/>
-      <c r="H52" s="3"/>
-    </row>
-    <row r="53" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G52" s="6">
+        <v>0</v>
+      </c>
+      <c r="K52" s="3"/>
+    </row>
+    <row r="53" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D53" s="4"/>
-      <c r="H53" s="3"/>
-    </row>
-    <row r="54" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G53" s="6">
+        <v>0</v>
+      </c>
+      <c r="K53" s="3"/>
+    </row>
+    <row r="54" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D54" s="4"/>
-      <c r="H54" s="3"/>
-    </row>
-    <row r="55" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G54" s="6">
+        <v>0</v>
+      </c>
+      <c r="K54" s="3"/>
+    </row>
+    <row r="55" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D55" s="4"/>
-      <c r="H55" s="3"/>
-    </row>
-    <row r="56" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G55" s="6">
+        <v>0</v>
+      </c>
+      <c r="K55" s="3"/>
+    </row>
+    <row r="56" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D56" s="4"/>
-      <c r="H56" s="3"/>
-    </row>
-    <row r="57" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G56" s="6">
+        <v>0</v>
+      </c>
+      <c r="K56" s="3"/>
+    </row>
+    <row r="57" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="4"/>
-      <c r="H57" s="3"/>
-    </row>
-    <row r="58" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G57" s="6">
+        <v>0</v>
+      </c>
+      <c r="K57" s="3"/>
+    </row>
+    <row r="58" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="4"/>
-      <c r="H58" s="3"/>
-    </row>
-    <row r="59" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G58" s="6">
+        <v>0</v>
+      </c>
+      <c r="K58" s="3"/>
+    </row>
+    <row r="59" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D59" s="4"/>
-      <c r="H59" s="3"/>
-    </row>
-    <row r="60" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G59" s="6">
+        <v>0</v>
+      </c>
+      <c r="K59" s="3"/>
+    </row>
+    <row r="60" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D60" s="4"/>
-      <c r="H60" s="3"/>
-    </row>
-    <row r="61" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G60" s="6">
+        <v>0</v>
+      </c>
+      <c r="K60" s="3"/>
+    </row>
+    <row r="61" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D61" s="4"/>
-      <c r="H61" s="3"/>
-    </row>
-    <row r="62" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G61" s="6">
+        <v>0</v>
+      </c>
+      <c r="K61" s="3"/>
+    </row>
+    <row r="62" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D62" s="4"/>
-      <c r="H62" s="3"/>
-    </row>
-    <row r="63" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G62" s="6">
+        <v>0</v>
+      </c>
+      <c r="K62" s="3"/>
+    </row>
+    <row r="63" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D63" s="4"/>
-      <c r="H63" s="3"/>
-    </row>
-    <row r="64" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G63" s="6">
+        <v>0</v>
+      </c>
+      <c r="K63" s="3"/>
+    </row>
+    <row r="64" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D64" s="4"/>
-      <c r="H64" s="3"/>
-    </row>
-    <row r="65" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G64" s="6">
+        <v>0</v>
+      </c>
+      <c r="K64" s="3"/>
+    </row>
+    <row r="65" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D65" s="4"/>
-      <c r="H65" s="3"/>
-    </row>
-    <row r="66" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G65" s="6">
+        <v>0</v>
+      </c>
+      <c r="K65" s="3"/>
+    </row>
+    <row r="66" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D66" s="4"/>
-      <c r="H66" s="3"/>
-    </row>
-    <row r="67" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G66" s="6">
+        <v>0</v>
+      </c>
+      <c r="K66" s="3"/>
+    </row>
+    <row r="67" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D67" s="4"/>
-      <c r="H67" s="3"/>
-    </row>
-    <row r="68" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G67" s="6">
+        <v>0</v>
+      </c>
+      <c r="K67" s="3"/>
+    </row>
+    <row r="68" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D68" s="4"/>
-      <c r="H68" s="3"/>
-    </row>
-    <row r="69" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G68" s="6">
+        <v>0</v>
+      </c>
+      <c r="K68" s="3"/>
+    </row>
+    <row r="69" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D69" s="4"/>
-      <c r="H69" s="3"/>
-    </row>
-    <row r="70" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G69" s="6">
+        <v>0</v>
+      </c>
+      <c r="K69" s="3"/>
+    </row>
+    <row r="70" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D70" s="4"/>
-      <c r="H70" s="3"/>
-    </row>
-    <row r="71" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G70" s="6">
+        <v>0</v>
+      </c>
+      <c r="K70" s="3"/>
+    </row>
+    <row r="71" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D71" s="4"/>
-      <c r="H71" s="3"/>
-    </row>
-    <row r="72" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G71" s="6">
+        <v>0</v>
+      </c>
+      <c r="K71" s="3"/>
+    </row>
+    <row r="72" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D72" s="4"/>
-      <c r="H72" s="3"/>
-    </row>
-    <row r="73" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G72" s="6">
+        <v>0</v>
+      </c>
+      <c r="K72" s="3"/>
+    </row>
+    <row r="73" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D73" s="4"/>
-      <c r="H73" s="3"/>
-    </row>
-    <row r="74" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G73" s="6">
+        <v>0</v>
+      </c>
+      <c r="K73" s="3"/>
+    </row>
+    <row r="74" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D74" s="4"/>
-      <c r="H74" s="3"/>
-    </row>
-    <row r="75" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G74" s="6">
+        <v>0</v>
+      </c>
+      <c r="K74" s="3"/>
+    </row>
+    <row r="75" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D75" s="4"/>
-      <c r="H75" s="3"/>
-    </row>
-    <row r="76" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G75" s="6">
+        <v>0</v>
+      </c>
+      <c r="K75" s="3"/>
+    </row>
+    <row r="76" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D76" s="4"/>
-      <c r="H76" s="3"/>
-    </row>
-    <row r="77" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G76" s="6">
+        <v>0</v>
+      </c>
+      <c r="K76" s="3"/>
+    </row>
+    <row r="77" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D77" s="4"/>
-      <c r="H77" s="3"/>
-    </row>
-    <row r="78" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G77" s="6">
+        <v>0</v>
+      </c>
+      <c r="K77" s="3"/>
+    </row>
+    <row r="78" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D78" s="4"/>
-      <c r="H78" s="3"/>
-    </row>
-    <row r="79" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G78" s="6">
+        <v>0</v>
+      </c>
+      <c r="K78" s="3"/>
+    </row>
+    <row r="79" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D79" s="4"/>
-      <c r="H79" s="3"/>
-    </row>
-    <row r="80" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G79" s="6">
+        <v>0</v>
+      </c>
+      <c r="K79" s="3"/>
+    </row>
+    <row r="80" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D80" s="4"/>
-      <c r="H80" s="3"/>
-    </row>
-    <row r="81" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G80" s="6">
+        <v>0</v>
+      </c>
+      <c r="K80" s="3"/>
+    </row>
+    <row r="81" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D81" s="4"/>
-      <c r="H81" s="3"/>
-    </row>
-    <row r="82" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G81" s="6">
+        <v>0</v>
+      </c>
+      <c r="K81" s="3"/>
+    </row>
+    <row r="82" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D82" s="4"/>
-      <c r="H82" s="3"/>
-    </row>
-    <row r="83" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G82" s="6">
+        <v>0</v>
+      </c>
+      <c r="K82" s="3"/>
+    </row>
+    <row r="83" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D83" s="4"/>
-      <c r="H83" s="3"/>
-    </row>
-    <row r="84" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G83" s="6">
+        <v>0</v>
+      </c>
+      <c r="K83" s="3"/>
+    </row>
+    <row r="84" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D84" s="4"/>
-      <c r="H84" s="3"/>
-    </row>
-    <row r="85" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G84" s="6">
+        <v>0</v>
+      </c>
+      <c r="K84" s="3"/>
+    </row>
+    <row r="85" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D85" s="4"/>
-      <c r="H85" s="3"/>
-    </row>
-    <row r="86" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G85" s="6">
+        <v>0</v>
+      </c>
+      <c r="K85" s="3"/>
+    </row>
+    <row r="86" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D86" s="4"/>
-      <c r="H86" s="3"/>
-    </row>
-    <row r="87" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G86" s="6">
+        <v>0</v>
+      </c>
+      <c r="K86" s="3"/>
+    </row>
+    <row r="87" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D87" s="4"/>
-      <c r="H87" s="3"/>
-    </row>
-    <row r="88" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G87" s="6">
+        <v>0</v>
+      </c>
+      <c r="K87" s="3"/>
+    </row>
+    <row r="88" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D88" s="4"/>
-      <c r="H88" s="3"/>
-    </row>
-    <row r="89" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G88" s="6">
+        <v>0</v>
+      </c>
+      <c r="K88" s="3"/>
+    </row>
+    <row r="89" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D89" s="4"/>
-      <c r="H89" s="3"/>
-    </row>
-    <row r="90" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G89" s="6">
+        <v>0</v>
+      </c>
+      <c r="K89" s="3"/>
+    </row>
+    <row r="90" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D90" s="4"/>
-      <c r="H90" s="3"/>
-    </row>
-    <row r="91" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G90" s="6">
+        <v>0</v>
+      </c>
+      <c r="K90" s="3"/>
+    </row>
+    <row r="91" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D91" s="4"/>
-      <c r="H91" s="3"/>
-    </row>
-    <row r="92" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G91" s="6">
+        <v>0</v>
+      </c>
+      <c r="K91" s="3"/>
+    </row>
+    <row r="92" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D92" s="4"/>
-      <c r="H92" s="3"/>
-    </row>
-    <row r="93" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G92" s="6">
+        <v>0</v>
+      </c>
+      <c r="K92" s="3"/>
+    </row>
+    <row r="93" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D93" s="4"/>
-      <c r="H93" s="3"/>
-    </row>
-    <row r="94" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G93" s="6">
+        <v>0</v>
+      </c>
+      <c r="K93" s="3"/>
+    </row>
+    <row r="94" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D94" s="4"/>
-      <c r="H94" s="3"/>
-    </row>
-    <row r="95" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G94" s="6">
+        <v>0</v>
+      </c>
+      <c r="K94" s="3"/>
+    </row>
+    <row r="95" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D95" s="4"/>
-      <c r="H95" s="3"/>
-    </row>
-    <row r="96" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G95" s="6">
+        <v>0</v>
+      </c>
+      <c r="K95" s="3"/>
+    </row>
+    <row r="96" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D96" s="4"/>
-      <c r="H96" s="3"/>
-    </row>
-    <row r="97" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G96" s="6">
+        <v>0</v>
+      </c>
+      <c r="K96" s="3"/>
+    </row>
+    <row r="97" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D97" s="4"/>
-      <c r="H97" s="3"/>
-    </row>
-    <row r="98" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G97" s="6">
+        <v>0</v>
+      </c>
+      <c r="K97" s="3"/>
+    </row>
+    <row r="98" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D98" s="4"/>
-      <c r="H98" s="3"/>
-    </row>
-    <row r="99" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G98" s="6">
+        <v>0</v>
+      </c>
+      <c r="K98" s="3"/>
+    </row>
+    <row r="99" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D99" s="4"/>
-      <c r="H99" s="3"/>
-    </row>
-    <row r="100" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G99" s="6">
+        <v>0</v>
+      </c>
+      <c r="K99" s="3"/>
+    </row>
+    <row r="100" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D100" s="4"/>
-      <c r="H100" s="3"/>
-    </row>
-    <row r="101" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G100" s="6">
+        <v>0</v>
+      </c>
+      <c r="K100" s="3"/>
+    </row>
+    <row r="101" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D101" s="4"/>
-      <c r="H101" s="3"/>
-    </row>
-    <row r="102" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G101" s="6">
+        <v>0</v>
+      </c>
+      <c r="K101" s="3"/>
+    </row>
+    <row r="102" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D102" s="4"/>
-      <c r="H102" s="3"/>
-    </row>
-    <row r="103" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G102" s="6">
+        <v>0</v>
+      </c>
+      <c r="K102" s="3"/>
+    </row>
+    <row r="103" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D103" s="4"/>
-      <c r="H103" s="3"/>
-    </row>
-    <row r="104" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G103" s="6">
+        <v>0</v>
+      </c>
+      <c r="K103" s="3"/>
+    </row>
+    <row r="104" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D104" s="4"/>
-      <c r="H104" s="3"/>
-    </row>
-    <row r="105" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G104" s="6">
+        <v>0</v>
+      </c>
+      <c r="K104" s="3"/>
+    </row>
+    <row r="105" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D105" s="4"/>
-      <c r="H105" s="3"/>
-    </row>
-    <row r="106" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G105" s="6">
+        <v>0</v>
+      </c>
+      <c r="K105" s="3"/>
+    </row>
+    <row r="106" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D106" s="4"/>
-      <c r="H106" s="3"/>
-    </row>
-    <row r="107" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G106" s="6">
+        <v>0</v>
+      </c>
+      <c r="K106" s="3"/>
+    </row>
+    <row r="107" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D107" s="4"/>
-      <c r="H107" s="3"/>
-    </row>
-    <row r="108" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G107" s="6">
+        <v>0</v>
+      </c>
+      <c r="K107" s="3"/>
+    </row>
+    <row r="108" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D108" s="4"/>
-      <c r="H108" s="3"/>
-    </row>
-    <row r="109" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G108" s="6">
+        <v>0</v>
+      </c>
+      <c r="K108" s="3"/>
+    </row>
+    <row r="109" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D109" s="4"/>
-      <c r="H109" s="3"/>
-    </row>
-    <row r="110" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G109" s="6">
+        <v>0</v>
+      </c>
+      <c r="K109" s="3"/>
+    </row>
+    <row r="110" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D110" s="4"/>
-      <c r="H110" s="3"/>
-    </row>
-    <row r="111" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G110" s="6">
+        <v>0</v>
+      </c>
+      <c r="K110" s="3"/>
+    </row>
+    <row r="111" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D111" s="4"/>
-      <c r="H111" s="3"/>
-    </row>
-    <row r="112" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G111" s="6">
+        <v>0</v>
+      </c>
+      <c r="K111" s="3"/>
+    </row>
+    <row r="112" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D112" s="4"/>
-      <c r="H112" s="3"/>
-    </row>
-    <row r="113" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G112" s="6">
+        <v>0</v>
+      </c>
+      <c r="K112" s="3"/>
+    </row>
+    <row r="113" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D113" s="4"/>
-      <c r="H113" s="3"/>
-    </row>
-    <row r="114" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G113" s="6">
+        <v>0</v>
+      </c>
+      <c r="K113" s="3"/>
+    </row>
+    <row r="114" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D114" s="4"/>
-      <c r="H114" s="3"/>
-    </row>
-    <row r="115" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G114" s="6">
+        <v>0</v>
+      </c>
+      <c r="K114" s="3"/>
+    </row>
+    <row r="115" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D115" s="4"/>
-      <c r="H115" s="3"/>
-    </row>
-    <row r="116" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G115" s="6">
+        <v>0</v>
+      </c>
+      <c r="K115" s="3"/>
+    </row>
+    <row r="116" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D116" s="4"/>
-      <c r="H116" s="3"/>
-    </row>
-    <row r="117" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G116" s="6">
+        <v>0</v>
+      </c>
+      <c r="K116" s="3"/>
+    </row>
+    <row r="117" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D117" s="4"/>
-      <c r="H117" s="3"/>
-    </row>
-    <row r="118" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G117" s="6">
+        <v>0</v>
+      </c>
+      <c r="K117" s="3"/>
+    </row>
+    <row r="118" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D118" s="4"/>
-      <c r="H118" s="3"/>
-    </row>
-    <row r="119" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G118" s="6">
+        <v>0</v>
+      </c>
+      <c r="K118" s="3"/>
+    </row>
+    <row r="119" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D119" s="4"/>
-      <c r="H119" s="3"/>
-    </row>
-    <row r="120" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G119" s="6">
+        <v>0</v>
+      </c>
+      <c r="K119" s="3"/>
+    </row>
+    <row r="120" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D120" s="4"/>
-      <c r="H120" s="3"/>
-    </row>
-    <row r="121" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G120" s="6">
+        <v>0</v>
+      </c>
+      <c r="K120" s="3"/>
+    </row>
+    <row r="121" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D121" s="4"/>
-      <c r="H121" s="3"/>
-    </row>
-    <row r="122" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G121" s="6">
+        <v>0</v>
+      </c>
+      <c r="K121" s="3"/>
+    </row>
+    <row r="122" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D122" s="4"/>
-      <c r="H122" s="3"/>
-    </row>
-    <row r="123" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G122" s="6">
+        <v>0</v>
+      </c>
+      <c r="K122" s="3"/>
+    </row>
+    <row r="123" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D123" s="4"/>
-      <c r="H123" s="3"/>
-    </row>
-    <row r="124" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G123" s="6">
+        <v>0</v>
+      </c>
+      <c r="K123" s="3"/>
+    </row>
+    <row r="124" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D124" s="4"/>
-      <c r="H124" s="3"/>
-    </row>
-    <row r="125" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G124" s="6">
+        <v>0</v>
+      </c>
+      <c r="K124" s="3"/>
+    </row>
+    <row r="125" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D125" s="4"/>
-      <c r="H125" s="3"/>
-    </row>
-    <row r="126" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G125" s="6">
+        <v>0</v>
+      </c>
+      <c r="K125" s="3"/>
+    </row>
+    <row r="126" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D126" s="4"/>
-      <c r="H126" s="3"/>
-    </row>
-    <row r="127" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G126" s="6">
+        <v>0</v>
+      </c>
+      <c r="K126" s="3"/>
+    </row>
+    <row r="127" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D127" s="4"/>
-      <c r="H127" s="3"/>
-    </row>
-    <row r="128" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G127" s="6">
+        <v>0</v>
+      </c>
+      <c r="K127" s="3"/>
+    </row>
+    <row r="128" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D128" s="4"/>
-      <c r="H128" s="3"/>
-    </row>
-    <row r="129" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G128" s="6">
+        <v>0</v>
+      </c>
+      <c r="K128" s="3"/>
+    </row>
+    <row r="129" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D129" s="4"/>
-      <c r="H129" s="3"/>
-    </row>
-    <row r="130" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G129" s="6">
+        <v>0</v>
+      </c>
+      <c r="K129" s="3"/>
+    </row>
+    <row r="130" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D130" s="4"/>
-      <c r="H130" s="3"/>
-    </row>
-    <row r="131" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G130" s="6">
+        <v>0</v>
+      </c>
+      <c r="K130" s="3"/>
+    </row>
+    <row r="131" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D131" s="4"/>
-      <c r="H131" s="3"/>
-    </row>
-    <row r="132" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G131" s="6">
+        <v>0</v>
+      </c>
+      <c r="K131" s="3"/>
+    </row>
+    <row r="132" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D132" s="4"/>
-      <c r="H132" s="3"/>
-    </row>
-    <row r="133" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G132" s="6">
+        <v>0</v>
+      </c>
+      <c r="K132" s="3"/>
+    </row>
+    <row r="133" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D133" s="4"/>
-      <c r="H133" s="3"/>
-    </row>
-    <row r="134" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G133" s="6">
+        <v>0</v>
+      </c>
+      <c r="K133" s="3"/>
+    </row>
+    <row r="134" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D134" s="4"/>
-      <c r="H134" s="3"/>
-    </row>
-    <row r="135" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G134" s="6">
+        <v>0</v>
+      </c>
+      <c r="K134" s="3"/>
+    </row>
+    <row r="135" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D135" s="4"/>
-      <c r="H135" s="3"/>
-    </row>
-    <row r="136" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G135" s="6">
+        <v>0</v>
+      </c>
+      <c r="K135" s="3"/>
+    </row>
+    <row r="136" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D136" s="4"/>
-      <c r="H136" s="3"/>
-    </row>
-    <row r="137" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G136" s="6">
+        <v>0</v>
+      </c>
+      <c r="K136" s="3"/>
+    </row>
+    <row r="137" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D137" s="4"/>
-      <c r="H137" s="3"/>
-    </row>
-    <row r="138" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G137" s="6">
+        <v>0</v>
+      </c>
+      <c r="K137" s="3"/>
+    </row>
+    <row r="138" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D138" s="4"/>
-      <c r="H138" s="3"/>
-    </row>
-    <row r="139" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G138" s="6">
+        <v>0</v>
+      </c>
+      <c r="K138" s="3"/>
+    </row>
+    <row r="139" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D139" s="4"/>
-      <c r="H139" s="3"/>
-    </row>
-    <row r="140" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G139" s="6">
+        <v>0</v>
+      </c>
+      <c r="K139" s="3"/>
+    </row>
+    <row r="140" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D140" s="4"/>
-      <c r="H140" s="3"/>
-    </row>
-    <row r="141" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G140" s="6">
+        <v>0</v>
+      </c>
+      <c r="K140" s="3"/>
+    </row>
+    <row r="141" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D141" s="4"/>
-      <c r="H141" s="3"/>
-    </row>
-    <row r="142" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G141" s="6">
+        <v>0</v>
+      </c>
+      <c r="K141" s="3"/>
+    </row>
+    <row r="142" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D142" s="4"/>
-      <c r="H142" s="3"/>
-    </row>
-    <row r="143" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G142" s="6">
+        <v>0</v>
+      </c>
+      <c r="K142" s="3"/>
+    </row>
+    <row r="143" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D143" s="4"/>
-      <c r="H143" s="3"/>
-    </row>
-    <row r="144" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G143" s="6">
+        <v>0</v>
+      </c>
+      <c r="K143" s="3"/>
+    </row>
+    <row r="144" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D144" s="4"/>
-      <c r="H144" s="3"/>
-    </row>
-    <row r="145" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G144" s="6">
+        <v>0</v>
+      </c>
+      <c r="K144" s="3"/>
+    </row>
+    <row r="145" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D145" s="4"/>
-      <c r="H145" s="3"/>
-    </row>
-    <row r="146" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G145" s="6">
+        <v>0</v>
+      </c>
+      <c r="K145" s="3"/>
+    </row>
+    <row r="146" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D146" s="4"/>
-      <c r="H146" s="3"/>
-    </row>
-    <row r="147" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G146" s="6">
+        <v>0</v>
+      </c>
+      <c r="K146" s="3"/>
+    </row>
+    <row r="147" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D147" s="4"/>
-      <c r="H147" s="3"/>
-    </row>
-    <row r="148" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G147" s="6">
+        <v>0</v>
+      </c>
+      <c r="K147" s="3"/>
+    </row>
+    <row r="148" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D148" s="4"/>
-      <c r="H148" s="3"/>
-    </row>
-    <row r="149" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G148" s="6">
+        <v>0</v>
+      </c>
+      <c r="K148" s="3"/>
+    </row>
+    <row r="149" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D149" s="4"/>
-      <c r="H149" s="3"/>
-    </row>
-    <row r="150" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G149" s="6">
+        <v>0</v>
+      </c>
+      <c r="K149" s="3"/>
+    </row>
+    <row r="150" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D150" s="4"/>
-      <c r="H150" s="3"/>
-    </row>
-    <row r="151" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G150" s="6">
+        <v>0</v>
+      </c>
+      <c r="K150" s="3"/>
+    </row>
+    <row r="151" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D151" s="4"/>
-      <c r="H151" s="3"/>
-    </row>
-    <row r="152" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G151" s="6">
+        <v>0</v>
+      </c>
+      <c r="K151" s="3"/>
+    </row>
+    <row r="152" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D152" s="4"/>
-      <c r="H152" s="3"/>
-    </row>
-    <row r="153" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G152" s="6">
+        <v>0</v>
+      </c>
+      <c r="K152" s="3"/>
+    </row>
+    <row r="153" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D153" s="4"/>
-      <c r="H153" s="3"/>
-    </row>
-    <row r="154" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G153" s="6">
+        <v>0</v>
+      </c>
+      <c r="K153" s="3"/>
+    </row>
+    <row r="154" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D154" s="4"/>
-      <c r="H154" s="3"/>
-    </row>
-    <row r="155" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G154" s="6">
+        <v>0</v>
+      </c>
+      <c r="K154" s="3"/>
+    </row>
+    <row r="155" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D155" s="4"/>
-      <c r="H155" s="3"/>
-    </row>
-    <row r="156" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G155" s="6">
+        <v>0</v>
+      </c>
+      <c r="K155" s="3"/>
+    </row>
+    <row r="156" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D156" s="4"/>
-      <c r="H156" s="3"/>
-    </row>
-    <row r="157" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G156" s="6">
+        <v>0</v>
+      </c>
+      <c r="K156" s="3"/>
+    </row>
+    <row r="157" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D157" s="4"/>
-      <c r="H157" s="3"/>
-    </row>
-    <row r="158" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G157" s="6">
+        <v>0</v>
+      </c>
+      <c r="K157" s="3"/>
+    </row>
+    <row r="158" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D158" s="4"/>
-      <c r="H158" s="3"/>
-    </row>
-    <row r="159" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G158" s="6">
+        <v>0</v>
+      </c>
+      <c r="K158" s="3"/>
+    </row>
+    <row r="159" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D159" s="4"/>
-      <c r="H159" s="3"/>
-    </row>
-    <row r="160" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G159" s="6">
+        <v>0</v>
+      </c>
+      <c r="K159" s="3"/>
+    </row>
+    <row r="160" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D160" s="4"/>
-      <c r="H160" s="3"/>
-    </row>
-    <row r="161" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G160" s="6">
+        <v>0</v>
+      </c>
+      <c r="K160" s="3"/>
+    </row>
+    <row r="161" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D161" s="4"/>
-      <c r="H161" s="3"/>
-    </row>
-    <row r="162" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G161" s="6">
+        <v>0</v>
+      </c>
+      <c r="K161" s="3"/>
+    </row>
+    <row r="162" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D162" s="4"/>
-      <c r="H162" s="3"/>
-    </row>
-    <row r="163" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G162" s="6">
+        <v>0</v>
+      </c>
+      <c r="K162" s="3"/>
+    </row>
+    <row r="163" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D163" s="4"/>
-      <c r="H163" s="3"/>
-    </row>
-    <row r="164" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G163" s="6">
+        <v>0</v>
+      </c>
+      <c r="K163" s="3"/>
+    </row>
+    <row r="164" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D164" s="4"/>
-      <c r="H164" s="3"/>
-    </row>
-    <row r="165" spans="4:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G164" s="6">
+        <v>0</v>
+      </c>
+      <c r="K164" s="3"/>
+    </row>
+    <row r="165" spans="4:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D165" s="4"/>
-      <c r="H165" s="3"/>
-    </row>
-    <row r="166" spans="4:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="G165" s="6">
+        <v>0</v>
+      </c>
+      <c r="K165" s="3"/>
+    </row>
+    <row r="166" spans="4:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>